<commit_message>
Features added: Success Counter Failure counter Ticket creation report Send report via mail
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\Jira Bot ReFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19979C14-35FC-4E30-AEED-D64348F5EB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37035BEB-E082-4AD9-8887-634A8EB2B6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -186,6 +186,33 @@
   </si>
   <si>
     <t>Jira_Login_Credentials</t>
+  </si>
+  <si>
+    <t>Email_Template_FilePath</t>
+  </si>
+  <si>
+    <t>Email_Template_Address</t>
+  </si>
+  <si>
+    <t>Data\Output\Jira Status Report.xlsx</t>
+  </si>
+  <si>
+    <t>Logs</t>
+  </si>
+  <si>
+    <t>A text document with the basic email template</t>
+  </si>
+  <si>
+    <t>Excel file that contains ticket creation logs</t>
+  </si>
+  <si>
+    <t>Jira Status Report worksheet name</t>
+  </si>
+  <si>
+    <t>JiraStatusReport</t>
+  </si>
+  <si>
+    <t>JiraStatusReportSheet</t>
   </si>
 </sst>
 </file>
@@ -572,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -652,63 +679,113 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>43</v>
-      </c>
+    <row r="6" spans="1:26" ht="14.5">
+      <c r="B6" s="2"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="2"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1675,10 +1752,16 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{3E6FC2BA-4496-4FD5-84E6-C42C8B0DA5B4}"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{3E6FC2BA-4496-4FD5-84E6-C42C8B0DA5B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2853,7 +2936,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2900,7 +2983,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added functionality:  Restrict dispatcher to run only once in case of system error  Save New Files to New Tickets folder and move them to Processed Tickets once dispatched to orchestrator
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\Jira Bot ReFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37035BEB-E082-4AD9-8887-634A8EB2B6B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6AF02A-67B5-44AA-9EE6-EE4DB75E23DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Attachment_Download_Folder</t>
   </si>
   <si>
-    <t>Data\Input</t>
-  </si>
-  <si>
     <t>Folder location for downloaded email attachment</t>
   </si>
   <si>
@@ -213,6 +210,18 @@
   </si>
   <si>
     <t>JiraStatusReportSheet</t>
+  </si>
+  <si>
+    <t>Folder containing excel files that have been dispatched to Orchestrator</t>
+  </si>
+  <si>
+    <t>ProcessedTicketsFolder</t>
+  </si>
+  <si>
+    <t>Data\Input\New Tickets</t>
+  </si>
+  <si>
+    <t>Data\Input\Processed Tickets</t>
   </si>
 </sst>
 </file>
@@ -602,7 +611,7 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -649,10 +658,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -673,7 +682,7 @@
         <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -685,7 +694,7 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>42</v>
@@ -704,10 +713,10 @@
         <v>44</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -717,13 +726,13 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -733,13 +742,13 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
@@ -748,13 +757,13 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -762,17 +771,27 @@
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2936,7 +2955,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2985,10 +3004,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>